<commit_message>
For PO Form Modify
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/PO_Mackarel.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/PO_Mackarel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290F7991-5BEB-41E8-B4DA-359D0B629E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576EE1C9-46EB-415C-AAB7-375F9C435A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,32 +55,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Quality Management System Requirements:  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General Condition: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quality:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packing &amp; Forwarding: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode of Payment: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment Terms: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode of Transport: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Delivery Time: </t>
-  </si>
-  <si>
-    <t>Any Other Requirements:</t>
   </si>
   <si>
     <t xml:space="preserve">GSTIN No. </t>
@@ -111,9 +86,6 @@
       </rPr>
       <t>Applicable version of material specifications / Drawing  / Applicable  Procedure &amp; Process Requirements  /  Inspection instruction / Traceability /  Other relevant technical data.</t>
     </r>
-  </si>
-  <si>
-    <t>PO Validity  :</t>
   </si>
   <si>
     <t>Note : If we receive material after due date then penalty of 0.5 % will be deducted per day from the total amount.</t>
@@ -241,6 +213,34 @@
   </si>
   <si>
     <t>Total amount in words : (USD : #ValueInWords  only)</t>
+  </si>
+  <si>
+    <t>General Condition: #GeneralCondition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quality Management System Requirements: #POQMSRequirement
+</t>
+  </si>
+  <si>
+    <t>Quality: #POQuality</t>
+  </si>
+  <si>
+    <t>Packing &amp; Forwarding: #POPackForward</t>
+  </si>
+  <si>
+    <t>Mode of Payment: #ModeOfPayment</t>
+  </si>
+  <si>
+    <t>Payment Terms: #PaymentTerms</t>
+  </si>
+  <si>
+    <t>Mode of Transport: #ModeOfTransport</t>
+  </si>
+  <si>
+    <t>Any Other Requirements: #AnyOtherRequirements</t>
+  </si>
+  <si>
+    <t>PO Validity  : #POValidity</t>
   </si>
 </sst>
 </file>
@@ -1366,8 +1366,8 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="78" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:H17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="78" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1385,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="126" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
@@ -1421,73 +1421,73 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="14" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="34"/>
       <c r="G4" s="16" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="18" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E5" s="61"/>
       <c r="F5" s="15"/>
       <c r="G5" s="87" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="84" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E6" s="61"/>
       <c r="F6" s="15"/>
       <c r="G6" s="89" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60"/>
       <c r="D7" s="62" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B8" s="64"/>
       <c r="C8" s="64"/>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="9" spans="1:8" s="13" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>3</v>
@@ -1520,7 +1520,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
@@ -1590,16 +1590,16 @@
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
       <c r="F16" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G16" s="29"/>
       <c r="H16" s="69" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="90" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B17" s="91"/>
       <c r="C17" s="91"/>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="19" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B19" s="101"/>
       <c r="C19" s="101"/>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="4"/>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="22" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="73" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B22" s="74"/>
       <c r="C22" s="75"/>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="23" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="4"/>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="24" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="77" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B24" s="78"/>
       <c r="C24" s="38"/>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="25" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B25" s="78"/>
       <c r="C25" s="38"/>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="26" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B26" s="78"/>
       <c r="C26" s="38"/>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="27" spans="1:11" s="31" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="38"/>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="28" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B28" s="78"/>
       <c r="C28" s="38"/>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="29" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="79" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B29" s="80"/>
       <c r="C29" s="81"/>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="30" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B30" s="38"/>
       <c r="C30" s="38"/>
@@ -1769,20 +1769,20 @@
     </row>
     <row r="31" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
       <c r="F31" s="35"/>
       <c r="G31" s="33" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H31" s="36" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1797,23 +1797,23 @@
     </row>
     <row r="33" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D33" s="43"/>
       <c r="E33" s="43"/>
       <c r="F33" s="42"/>
       <c r="G33" s="42" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H33" s="44"/>
     </row>
     <row r="34" spans="1:9" s="31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="45" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="35" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="88" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -1858,7 +1858,7 @@
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="52"/>
       <c r="B38" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -1870,10 +1870,10 @@
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
       <c r="B39" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>

</xml_diff>